<commit_message>
Add tmux command into shortcut table
</commit_message>
<xml_diff>
--- a/shortcuts/win-mac-dev-util.xlsx
+++ b/shortcuts/win-mac-dev-util.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i348151/workspace/github/tools/shortcuts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i348151/workspace/github/computer.tools/shortcuts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E866AF56-A910-404F-833A-DB6C9CE70C85}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDE54B92-8568-6C4E-A56B-6960D1535546}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16500" xr2:uid="{BBC1CA9D-A7C2-A04E-A47E-88F2ED23C0E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$H$29</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>Intellij Idea</t>
   </si>
@@ -114,13 +117,6 @@
     <t>Win + Shift + S</t>
   </si>
   <si>
-    <t>Screenshot Rectangle 
-to Clipboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> -&gt; Paste to Paint</t>
-  </si>
-  <si>
     <t xml:space="preserve">Shift + F10 </t>
   </si>
   <si>
@@ -149,12 +145,6 @@
   </si>
   <si>
     <t>Refactor</t>
-  </si>
-  <si>
-    <t>Ctrl + Alt + Left</t>
-  </si>
-  <si>
-    <t>Back</t>
   </si>
   <si>
     <t xml:space="preserve">Ctrl + Alt +N </t>
@@ -263,7 +253,49 @@
     <t>Quick grep files</t>
   </si>
   <si>
-    <t>rg.         [scoop]</t>
+    <t>Ctrl + Alt + Left/Right</t>
+  </si>
+  <si>
+    <t>Ctrl + Shift + Backspace</t>
+  </si>
+  <si>
+    <t>Navigate back/forword</t>
+  </si>
+  <si>
+    <t>Navigate to last edit location</t>
+  </si>
+  <si>
+    <t>Tmux</t>
+  </si>
+  <si>
+    <t>tmux new -s abc</t>
+  </si>
+  <si>
+    <t>tmux ls</t>
+  </si>
+  <si>
+    <t>tmux attach-session -t abc</t>
+  </si>
+  <si>
+    <t>* name parentfolder\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                -&gt; to Clipboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        -&gt; Paste to Paint</t>
+  </si>
+  <si>
+    <t>Wox open folder</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screenshot Rectangle </t>
+  </si>
+  <si>
+    <t xml:space="preserve">      -&gt; to select json body)</t>
+  </si>
+  <si>
+    <t>rg          [scoop]</t>
   </si>
 </sst>
 </file>
@@ -302,7 +334,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -328,11 +360,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -347,13 +388,19 @@
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -671,24 +718,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51D02C41-EE36-3547-A2D0-C727C78DBCF1}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="125" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="70" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.83203125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12" style="1" customWidth="1"/>
     <col min="2" max="2" width="24.1640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="1" style="1" customWidth="1"/>
     <col min="5" max="5" width="0.1640625" style="5" customWidth="1"/>
     <col min="6" max="6" width="1" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.6640625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="27.5" style="1" customWidth="1"/>
     <col min="9" max="16384" width="21.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" s="2" customFormat="1" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -700,9 +747,9 @@
       </c>
       <c r="H1" s="6"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
@@ -717,12 +764,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -731,7 +778,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
@@ -745,7 +792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>19</v>
       </c>
@@ -759,9 +806,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>5</v>
@@ -773,7 +820,13 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="G7" s="1" t="s">
         <v>15</v>
       </c>
@@ -781,13 +834,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="8" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="G8" s="1" t="s">
         <v>16</v>
       </c>
@@ -795,216 +842,240 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="G9" s="1" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>43</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G13" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="7"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>39</v>
-      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G12" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
         <v>34</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>29</v>
+      <c r="G14" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G15" s="9"/>
+        <v>45</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="H15" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G18" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="1" t="s">
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="7"/>
+    </row>
+    <row r="22" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10"/>
+      <c r="B23" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="H19" s="7"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G20" s="1" t="s">
+    </row>
+    <row r="24" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="1" t="s">
+      <c r="H25" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="H26" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H22" s="7"/>
-    </row>
-    <row r="23" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="11"/>
-      <c r="B23" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="11"/>
-      <c r="B24" s="10"/>
-      <c r="C24" s="8"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>72</v>
-      </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="A23:A24"/>
-  </mergeCells>
   <pageMargins left="0.6" right="0.6" top="0.6" bottom="0.6" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>